<commit_message>
Added missing UID's (Bar Codes)
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE01ISSP_00006.xlsx
+++ b/deployment/Omaha_Cal_Info_CE01ISSP_00006.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="465" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
   </bookViews>
@@ -20,12 +25,12 @@
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$I$50</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="116">
   <si>
     <t>Ref Des</t>
   </si>
@@ -384,6 +389,9 @@
   <si>
     <t>[15.33333333, 16.95833333, 16.00000000, 17.12500000, 18.66666667, 17.33333333, 17.87500000, 16.91666667, 17.79166667, 21.33333333, 22.08333333, 41.16666667, 106.16666667, 321.16666667, 868.16666667, 1948.00000000, 3595.83333333, 5565.16666667, 7493.87500000, 9186.66666667, 10579.04166667, 11766.70833333, 12861.29166667, 13920.20833333, 15037.37500000, 16252.41666667, 17616.16666667, 19154.00000000, 20930.16666667, 22960.95833333, 25281.00000000, 27897.12500000, 30773.37500000, 33841.29166667, 36997.66666667, 40051.29166667, 42804.87500000, 45057.70833333, 46541.87500000, 47212.25000000, 46959.70833333, 45954.12500000, 44341.12500000, 42396.20833333, 40325.66666667, 38362.33333333, 36589.12500000, 35103.70833333, 33944.41666667, 33105.41666667, 32591.12500000, 32424.29166667, 32517.00000000, 32917.08333333, 33608.20833333, 34541.95833333, 35691.54166667, 37086.29166667, 38666.00000000, 40417.66666667, 42294.66666667, 44213.66666667, 46168.45833333, 48045.91666667, 49672.00000000, 51008.33333333, 51950.33333333, 52352.20833333, 52237.54166667, 51601.79166667, 50472.50000000, 48984.37500000, 47182.83333333, 45300.62500000, 43364.33333333, 41478.70833333, 39686.70833333, 38080.20833333, 36630.16666667, 35338.00000000, 34240.04166667, 33286.95833333, 32480.50000000, 31880.87500000, 31391.66666667, 31083.75000000, 30918.37500000, 30876.33333333, 31000.75000000, 31263.08333333, 31653.37500000, 32173.50000000, 32828.50000000, 33571.08333333, 34388.62500000, 35304.70833333, 36229.12500000, 37116.20833333, 37979.45833333, 38715.75000000, 39290.08333333, 39590.62500000, 39672.54166667, 39454.79166667, 38916.20833333, 38103.20833333, 37093.91666667, 35911.45833333, 34593.75000000, 33233.04166667, 31873.66666667, 30567.75000000, 29329.75000000, 28198.79166667, 27169.33333333, 26254.00000000, 25445.66666667, 24772.45833333, 24214.66666667, 23781.95833333, 23465.08333333, 23260.75000000, 23157.91666667, 23180.33333333, 23282.00000000, 23467.16666667, 23765.87500000, 24146.58333333, 24599.33333333, 25135.12500000, 25753.87500000, 26438.33333333, 27179.70833333, 27955.95833333, 28821.91666667, 29730.12500000, 30657.83333333, 31605.25000000, 32589.41666667, 33562.37500000, 34503.29166667, 35424.91666667, 36265.50000000, 37070.20833333, 37761.83333333, 38312.58333333, 38756.87500000, 39061.45833333, 39191.62500000, 39196.37500000, 39083.95833333, 38785.00000000, 38376.45833333, 37884.54166667, 37258.87500000, 36549.66666667, 35763.04166667, 34914.08333333, 34056.95833333, 33171.29166667, 32277.91666667, 31422.83333333, 30584.25000000, 29776.75000000, 29012.00000000, 28304.29166667, 27582.58333333, 26907.08333333, 26216.87500000, 25567.91666667, 24937.66666667, 24311.45833333, 23691.41666667, 23116.75000000, 22572.16666667, 22097.87500000, 21691.79166667, 21322.62500000, 21015.45833333, 20774.66666667, 20557.16666667, 20400.04166667, 20307.62500000, 20233.29166667, 20176.79166667, 20147.83333333, 20114.91666667, 20103.66666667, 20078.33333333, 20060.50000000, 20046.29166667, 20012.00000000, 19958.41666667, 19925.04166667, 19904.04166667, 19897.37500000, 19904.75000000, 19907.00000000, 19911.33333333, 19912.25000000, 19934.70833333, 19966.12500000, 20009.29166667, 20043.29166667, 20073.75000000, 20102.25000000, 20116.12500000, 20131.62500000, 20135.12500000, 20104.50000000, 20035.95833333, 19986.04166667, 19890.91666667, 19753.33333333, 19610.33333333, 19413.04166667, 19216.00000000, 18974.91666667, 18727.50000000, 18451.45833333, 18201.04166667, 17930.37500000, 17664.54166667, 17348.70833333, 16953.75000000, 16539.66666667, 16113.50000000, 15717.62500000, 15370.25000000, 15052.66666667, 14746.45833333, 14492.16666667, 14246.08333333, 14015.75000000, 13806.58333333, 13628.16666667, 13522.66666667, 13402.75000000, 13209.50000000, 12944.75000000, 12689.58333333, 12471.37500000, 12274.95833333, 12094.75000000, 11926.79166667, 11784.20833333, 11674.00000000, 11604.41666667, 11542.00000000, 11457.00000000, 11272.12500000, 10958.87500000, 10476.79166667, 9838.54166667, 9019.58333333, 7903.91666667]</t>
   </si>
+  <si>
+    <t>OL000617</t>
+  </si>
 </sst>
 </file>
 
@@ -626,7 +634,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,12 +673,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1282,7 +1284,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1392,7 +1394,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="34" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="516">
@@ -1919,6 +1920,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2265,7 +2269,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H8"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2328,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
+      <c r="A2" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="B2" s="29" t="s">
         <v>68</v>
       </c>
@@ -2459,9 +2465,9 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,14 +2526,16 @@
       <c r="A3" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C3" s="19" t="s">
         <v>112</v>
       </c>
       <c r="D3" s="20">
         <v>6</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="7" t="s">
         <v>103</v>
       </c>
       <c r="F3" s="36" t="s">
@@ -2555,7 +2563,9 @@
       <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="49"/>
+      <c r="B5" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C5" s="19" t="s">
         <v>112</v>
       </c>
@@ -2582,7 +2592,9 @@
       <c r="A6" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="49"/>
+      <c r="B6" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C6" s="40" t="s">
         <v>112</v>
       </c>
@@ -2620,7 +2632,9 @@
       <c r="A8" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="49"/>
+      <c r="B8" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C8" s="19" t="s">
         <v>112</v>
       </c>
@@ -2647,7 +2661,9 @@
       <c r="A9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="49"/>
+      <c r="B9" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C9" s="40" t="s">
         <v>112</v>
       </c>
@@ -2674,7 +2690,9 @@
       <c r="A10" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="49"/>
+      <c r="B10" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C10" s="40" t="s">
         <v>112</v>
       </c>
@@ -2701,7 +2719,9 @@
       <c r="A11" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="49"/>
+      <c r="B11" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C11" s="40" t="s">
         <v>112</v>
       </c>
@@ -2739,7 +2759,9 @@
       <c r="A13" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="49"/>
+      <c r="B13" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C13" s="19" t="s">
         <v>112</v>
       </c>
@@ -2766,7 +2788,9 @@
       <c r="A14" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="49"/>
+      <c r="B14" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C14" s="40" t="s">
         <v>112</v>
       </c>
@@ -2793,7 +2817,9 @@
       <c r="A15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="49"/>
+      <c r="B15" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C15" s="40" t="s">
         <v>112</v>
       </c>
@@ -2820,7 +2846,9 @@
       <c r="A16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C16" s="40" t="s">
         <v>112</v>
       </c>
@@ -2847,7 +2875,9 @@
       <c r="A17" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C17" s="40" t="s">
         <v>112</v>
       </c>
@@ -2874,7 +2904,9 @@
       <c r="A18" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C18" s="40" t="s">
         <v>112</v>
       </c>
@@ -2901,7 +2933,9 @@
       <c r="A19" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="49"/>
+      <c r="B19" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C19" s="40" t="s">
         <v>112</v>
       </c>
@@ -2928,7 +2962,9 @@
       <c r="A20" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="49"/>
+      <c r="B20" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C20" s="40" t="s">
         <v>112</v>
       </c>
@@ -2955,7 +2991,9 @@
       <c r="A21" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="49"/>
+      <c r="B21" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C21" s="40" t="s">
         <v>112</v>
       </c>
@@ -2982,7 +3020,9 @@
       <c r="A22" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="49"/>
+      <c r="B22" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C22" s="40" t="s">
         <v>112</v>
       </c>
@@ -3020,7 +3060,9 @@
       <c r="A24" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="49"/>
+      <c r="B24" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C24" s="19" t="s">
         <v>112</v>
       </c>
@@ -3047,7 +3089,9 @@
       <c r="A25" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="49"/>
+      <c r="B25" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C25" s="40" t="s">
         <v>112</v>
       </c>
@@ -3074,7 +3118,9 @@
       <c r="A26" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="49"/>
+      <c r="B26" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C26" s="40" t="s">
         <v>112</v>
       </c>
@@ -3101,7 +3147,9 @@
       <c r="A27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="49"/>
+      <c r="B27" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C27" s="40" t="s">
         <v>112</v>
       </c>
@@ -3128,7 +3176,9 @@
       <c r="A28" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="49"/>
+      <c r="B28" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C28" s="40" t="s">
         <v>112</v>
       </c>
@@ -3155,7 +3205,9 @@
       <c r="A29" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="49"/>
+      <c r="B29" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C29" s="40" t="s">
         <v>112</v>
       </c>
@@ -3182,7 +3234,9 @@
       <c r="A30" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="49"/>
+      <c r="B30" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C30" s="40" t="s">
         <v>112</v>
       </c>
@@ -3198,7 +3252,7 @@
       <c r="G30" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="50" t="s">
+      <c r="H30" s="49" t="s">
         <v>114</v>
       </c>
       <c r="I30" s="16" t="s">
@@ -3220,7 +3274,9 @@
       <c r="A32" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="49"/>
+      <c r="B32" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C32" s="19" t="s">
         <v>112</v>
       </c>
@@ -3245,7 +3301,9 @@
       <c r="A33" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="49"/>
+      <c r="B33" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C33" s="40" t="s">
         <v>112</v>
       </c>
@@ -3270,7 +3328,9 @@
       <c r="A34" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="49"/>
+      <c r="B34" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C34" s="40" t="s">
         <v>112</v>
       </c>
@@ -3295,7 +3355,9 @@
       <c r="A35" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="49"/>
+      <c r="B35" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C35" s="40" t="s">
         <v>112</v>
       </c>
@@ -3320,7 +3382,9 @@
       <c r="A36" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="49"/>
+      <c r="B36" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C36" s="40" t="s">
         <v>112</v>
       </c>
@@ -3345,7 +3409,9 @@
       <c r="A37" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="49"/>
+      <c r="B37" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C37" s="40" t="s">
         <v>112</v>
       </c>
@@ -3370,7 +3436,9 @@
       <c r="A38" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="49"/>
+      <c r="B38" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C38" s="40" t="s">
         <v>112</v>
       </c>
@@ -3395,7 +3463,9 @@
       <c r="A39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="49"/>
+      <c r="B39" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C39" s="40" t="s">
         <v>112</v>
       </c>
@@ -3431,7 +3501,9 @@
       <c r="A41" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="49"/>
+      <c r="B41" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C41" s="19" t="s">
         <v>112</v>
       </c>
@@ -3458,7 +3530,9 @@
       <c r="A42" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="49"/>
+      <c r="B42" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C42" s="40" t="s">
         <v>112</v>
       </c>
@@ -3485,7 +3559,9 @@
       <c r="A43" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C43" s="40" t="s">
         <v>112</v>
       </c>
@@ -3521,7 +3597,9 @@
       <c r="A45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="49"/>
+      <c r="B45" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C45" s="19" t="s">
         <v>112</v>
       </c>
@@ -3546,7 +3624,9 @@
       <c r="A46" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="49"/>
+      <c r="B46" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C46" s="40" t="s">
         <v>112</v>
       </c>
@@ -3571,7 +3651,9 @@
       <c r="A47" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="49"/>
+      <c r="B47" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C47" s="40" t="s">
         <v>112</v>
       </c>
@@ -3607,7 +3689,9 @@
       <c r="A49" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="49"/>
+      <c r="B49" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C49" s="19" t="s">
         <v>112</v>
       </c>
@@ -3634,7 +3718,9 @@
       <c r="A50" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="49"/>
+      <c r="B50" s="49" t="s">
+        <v>115</v>
+      </c>
       <c r="C50" s="40" t="s">
         <v>112</v>
       </c>

</xml_diff>